<commit_message>
update documentation to equal submitted slides
</commit_message>
<xml_diff>
--- a/data/queries.xlsx
+++ b/data/queries.xlsx
@@ -1,19 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/haukeroggenkamp/dev/mvfw/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE7E20C3-E283-A64B-B48F-42BAFCD1D405}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE14C0D9-1004-8E46-BCDF-EAB962BEF55B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1540" windowWidth="28040" windowHeight="17360" xr2:uid="{D67AD692-4747-BF4F-8789-DAB8BB220208}"/>
+    <workbookView xWindow="3340" yWindow="-19260" windowWidth="28040" windowHeight="17360" activeTab="1" xr2:uid="{D67AD692-4747-BF4F-8789-DAB8BB220208}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="MVFW" sheetId="1" r:id="rId1"/>
+    <sheet name="TimeFrames" sheetId="5" r:id="rId2"/>
+    <sheet name="MFW" sheetId="3" r:id="rId3"/>
+    <sheet name="NYFW" sheetId="2" r:id="rId4"/>
+    <sheet name="Tabelle4" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,15 +40,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="180">
   <si>
     <t>Brand</t>
   </si>
   <si>
     <t>Username</t>
-  </si>
-  <si>
-    <t>Query Parameters</t>
   </si>
   <si>
     <t>Query</t>
@@ -215,13 +216,379 @@
   </si>
   <si>
     <t xml:space="preserve">Just another Machine OG #AR #VR Augmentor, Creator, Builder, DirectorInk Illustrator meets #3D #Cryptoart &amp; #Games #SuperRare #Makersplace </t>
+  </si>
+  <si>
+    <t>twint -u tommyhilfiger -s "mfw OR (Milan Fashion Week)"  --lang "en" -o dev/mvfw/data/milanfw/tommyhilfiger.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u forever21 -s "mfw OR (Milan Fashion Week)"  --lang "en" -o dev/mvfw/data/milanfw/forever21.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u esteelauder -s "mfw OR (Milan Fashion Week)" --lang "en" -o dev/mvfw/data/milanfw/esteelauder.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u KarlLagerfeld -s "mfw OR (Milan Fashion Week)" --lang "en" -o dev/mvfw/data/milanfw/KarlLagerfeld.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u McQueen -s "mfw OR (Milan Fashion Week)" --lang "en" -o dev/mvfw/data/milanfw/McQueen.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u dkny -s "mfw OR (Milan Fashion Week)"  --lang "en" -o dev/mvfw/data/milanfw/dkny.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u dressxcom -s "mfw OR (Milan Fashion Week)" --lang "en" -o dev/mvfw/data/milanfw/dressxcom.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u dolcegabbana -s "mfw OR (Milan Fashion Week)"  --lang "en" -o dev/mvfw/data/milanfw/dolcegabbana.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u EtroOfficial -s "mfw OR (Milan Fashion Week)"  --lang "en" -o dev/mvfw/data/milanfw/EtroOfficial.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u FranckMuller -s "mfw OR (Milan Fashion Week)"  --lang "en" -o dev/mvfw/data/milanfw/FranckMuller.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u Selfridges -s "mfw OR (Milan Fashion Week)"  --lang "en" -o dev/mvfw/data/milanfw/Selfridges.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u Bulova -s "mfw OR (Milan Fashion Week)"  --lang "en" -o dev/mvfw/data/milanfw/Bulova.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u PacoRabanne -s "mfw OR (Milan Fashion Week)"  --lang "en" -o dev/mvfw/data/milanfw/PacoRabanne.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u ArtistVasarely -s "mfw OR (Milan Fashion Week)"  --lang "en" -o dev/mvfw/data/milanfw/ArtistVasarely.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u PUMA -s "mfw OR (Milan Fashion Week)"  --lang "en" -o dev/mvfw/data/milanfw/PUMA.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u PerryEllis -s "mfw OR (Milan Fashion Week)" --lang "en" -o dev/mvfw/data/milanfw/PerryEllis.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u Fred_Segal -s "mfw OR (Milan Fashion Week)"  --lang "en" -o dev/mvfw/data/milanfw/Fred_Segal.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u VAULTswiss -s "mfw OR (Milan Fashion Week)"  --lang "en" -o dev/mvfw/data/milanfw/VAULTswiss.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u MissJAlexander -s "mfw OR (Milan Fashion Week)"  --lang "en" -o dev/mvfw/data/milanfw/MissJAlexander.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u marc0matic -s "mfw OR (Milan Fashion Week)" --lang "en" -o dev/mvfw/data/milanfw/marc0matic.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u Charles_Keith -s "mfw OR (Milan Fashion Week)"  --lang "en" -o dev/mvfw/data/milanfw/Charles_Keith.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u priveporter -s "mfw OR (Milan Fashion Week)"  --lang "en" -o dev/mvfw/data/milanfw/priveporter.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u philipp_plein -s "mfw OR (Milan Fashion Week)"  --lang "en" -o dev/mvfw/data/milanfw/philipp_plein.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u ElieSaabWorld -s "mfw OR (Milan Fashion Week)" --lang "en" -o dev/mvfw/data/milanfw/ElieSaabWorld.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u HoganBrand -s "mfw OR (Milan Fashion Week)" --lang "en" -o dev/mvfw/data/milanfw/HoganBrand.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u IOCNFTs -s "mfw OR (Milan Fashion Week)"  --lang "en" -o dev/mvfw/data/milanfw/IOCNFTs.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u dundaslondon -s "mfw OR (Milan Fashion Week)"  --lang "en" -o dev/mvfw/data/milanfw/dundaslondon.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u tommyhilfiger -s "nyfw OR (New York Fashion Week)"  --since "2022-09-09" --until "2022-09-14" --lang "en" -o dev/mvfw/data/nyfw/tommyhilfiger.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u forever21 -s "nyfw OR (New York Fashion Week)"  --since "2022-09-09" --until "2022-09-14" --lang "en" -o dev/mvfw/data/nyfw/forever21.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u esteelauder -s "nyfw OR (New York Fashion Week)"  --since "2022-09-09" --until "2022-09-14" --lang "en" -o dev/mvfw/data/nyfw/esteelauder.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u KarlLagerfeld -s "nyfw OR (New York Fashion Week)"  --since "2022-09-09" --until "2022-09-14" --lang "en" -o dev/mvfw/data/nyfw/KarlLagerfeld.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u McQueen -s "nyfw OR (New York Fashion Week)"  --since "2022-09-09" --until "2022-09-14" --lang "en" -o dev/mvfw/data/nyfw/McQueen.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u dkny -s "nyfw OR (New York Fashion Week)"  --since "2022-09-09" --until "2022-09-14" --lang "en" -o dev/mvfw/data/nyfw/dkny.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u dressxcom -s "nyfw OR (New York Fashion Week)"  --since "2022-09-09" --until "2022-09-14" --lang "en" -o dev/mvfw/data/nyfw/dressxcom.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u dolcegabbana -s "nyfw OR (New York Fashion Week)"  --since "2022-09-09" --until "2022-09-14" --lang "en" -o dev/mvfw/data/nyfw/dolcegabbana.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u EtroOfficial -s "nyfw OR (New York Fashion Week)"  --since "2022-09-09" --until "2022-09-14" --lang "en" -o dev/mvfw/data/nyfw/EtroOfficial.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u FranckMuller -s "nyfw OR (New York Fashion Week)"  --since "2022-09-09" --until "2022-09-14" --lang "en" -o dev/mvfw/data/nyfw/FranckMuller.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u Selfridges -s "nyfw OR (New York Fashion Week)"  --since "2022-09-09" --until "2022-09-14" --lang "en" -o dev/mvfw/data/nyfw/Selfridges.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u Bulova -s "nyfw OR (New York Fashion Week)"  --since "2022-09-09" --until "2022-09-14" --lang "en" -o dev/mvfw/data/nyfw/Bulova.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u PacoRabanne -s "nyfw OR (New York Fashion Week)"  --since "2022-09-09" --until "2022-09-14" --lang "en" -o dev/mvfw/data/nyfw/PacoRabanne.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u ArtistVasarely -s "nyfw OR (New York Fashion Week)"  --since "2022-09-09" --until "2022-09-14" --lang "en" -o dev/mvfw/data/nyfw/ArtistVasarely.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u PUMA -s "nyfw OR (New York Fashion Week)"  --since "2022-09-09" --until "2022-09-14" --lang "en" -o dev/mvfw/data/nyfw/PUMA.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u PerryEllis -s "nyfw OR (New York Fashion Week)"  --since "2022-09-09" --until "2022-09-14" --lang "en" -o dev/mvfw/data/nyfw/PerryEllis.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u Fred_Segal -s "nyfw OR (New York Fashion Week)"  --since "2022-09-09" --until "2022-09-14" --lang "en" -o dev/mvfw/data/nyfw/Fred_Segal.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u VAULTswiss -s "nyfw OR (New York Fashion Week)"  --since "2022-09-09" --until "2022-09-14" --lang "en" -o dev/mvfw/data/nyfw/VAULTswiss.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u MissJAlexander -s "nyfw OR (New York Fashion Week)"  --since "2022-09-09" --until "2022-09-14" --lang "en" -o dev/mvfw/data/nyfw/MissJAlexander.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u marc0matic -s "nyfw OR (New York Fashion Week)"  --since "2022-09-09" --until "2022-09-14" --lang "en" -o dev/mvfw/data/nyfw/marc0matic.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u Charles_Keith -s "nyfw OR (New York Fashion Week)"  --since "2022-09-09" --until "2022-09-14" --lang "en" -o dev/mvfw/data/nyfw/Charles_Keith.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u priveporter -s "nyfw OR (New York Fashion Week)"  --since "2022-09-09" --until "2022-09-14" --lang "en" -o dev/mvfw/data/nyfw/priveporter.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u philipp_plein -s "nyfw OR (New York Fashion Week)"  --since "2022-09-09" --until "2022-09-14" --lang "en" -o dev/mvfw/data/nyfw/philipp_plein.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u ElieSaabWorld -s "nyfw OR (New York Fashion Week)"  --since "2022-09-09" --until "2022-09-14" --lang "en" -o dev/mvfw/data/nyfw/ElieSaabWorld.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u HoganBrand -s "nyfw OR (New York Fashion Week)"  --since "2022-09-09" --until "2022-09-14" --lang "en" -o dev/mvfw/data/nyfw/HoganBrand.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u IOCNFTs -s "nyfw OR (New York Fashion Week)"  --since "2022-09-09" --until "2022-09-14" --lang "en" -o dev/mvfw/data/nyfw/IOCNFTs.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u dundaslondon -s "nyfw OR (New York Fashion Week)"  --since "2022-09-09" --until "2022-09-14" --lang "en" -o dev/mvfw/data/nyfw/dundaslondon.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u beautyller -s "mvfw OR (Metaverse Fashion Week)" --since "2022-02-23" --until "2022-04-24" --lang "en" -o dev/mvfw/data/contentphysical/beautyller.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u eneftyfashion -s "mvfw OR (Metaverse Fashion Week)" --since "2022-02-23" --until "2022-04-24" --lang "en" -o dev/mvfw/data/contentphysical/eneftyfashion.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u arentfoxfashion -s "mvfw OR (Metaverse Fashion Week)" --since "2022-02-23" --until "2022-04-24" --lang "en" -o dev/mvfw/data/contentphysical/arentfoxfashion.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u thefashionlaw -s "mvfw OR (Metaverse Fashion Week)" --since "2022-02-23" --until "2022-04-24" --lang "en" -o dev/mvfw/data/contentphysical/thefashionlaw.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u fibre2fashion -s "mvfw OR (Metaverse Fashion Week)" --since "2022-02-23" --until "2022-04-24" --lang "en" -o dev/mvfw/data/contentphysical/fibre2fashion.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u fashioningip -s "mvfw OR (Metaverse Fashion Week)" --since "2022-02-23" --until "2022-04-24" --lang "en" -o dev/mvfw/data/contentphysical/fashioningip.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u maghanmcd -s "mvfw OR (Metaverse Fashion Week)" --since "2022-02-23" --until "2022-04-24" --lang "en" -o dev/mvfw/data/contentphysical/maghanmcd.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u luxurycruxx -s "mvfw OR (Metaverse Fashion Week)" --since "2022-02-23" --until "2022-04-24" --lang "en" -o dev/mvfw/data/contentphysical/luxurycruxx.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u fashionabc_ -s "mvfw OR (Metaverse Fashion Week)" --since "2022-02-23" --until "2022-04-24" --lang "en" -o dev/mvfw/data/contentphysical/fashionabc_.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u highfashiondose -s "mvfw OR (Metaverse Fashion Week)" --since "2022-02-23" --until "2022-04-24" --lang "en" -o dev/mvfw/data/contentphysical/highfashiondose.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u indyfashion -s "mvfw OR (Metaverse Fashion Week)" --since "2022-02-23" --until "2022-04-24" --lang "en" -o dev/mvfw/data/contentphysical/indyfashion.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u metafashionh -s "mvfw OR (Metaverse Fashion Week)" --since "2022-02-23" --until "2022-04-24" --lang "en" -o dev/mvfw/data/contentphysical/metafashionh.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u fashionunitednz -s "mvfw OR (Metaverse Fashion Week)" --since "2022-02-23" --until "2022-04-24" --lang "en" -o dev/mvfw/data/contentphysical/fashionunitednz.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u cppluxury -s "mvfw OR (Metaverse Fashion Week)" --since "2022-02-23" --until "2022-04-24" --lang "en" -o dev/mvfw/data/contentphysical/cppluxury.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u diamondhandbag -s "mvfw OR (Metaverse Fashion Week)" --since "2022-02-23" --until "2022-04-24" --lang "en" -o dev/mvfw/data/contentphysical/diamondhandbag.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u 360fashion -s "mvfw OR (Metaverse Fashion Week)" --since "2022-02-23" --until "2022-04-24" --lang "en" -o dev/mvfw/data/contentphysical/360fashion.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u faze_fashion -s "mvfw OR (Metaverse Fashion Week)" --since "2022-02-23" --until "2022-04-24" --lang "en" -o dev/mvfw/data/contentphysical/faze_fashion.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u forbeslife -s "mvfw OR (Metaverse Fashion Week)" --since "2022-02-23" --until "2022-04-24" --lang "en" -o dev/mvfw/data/contentphysical/forbeslife.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u jomsyfashion -s "mvfw OR (Metaverse Fashion Week)" --since "2022-02-23" --until "2022-04-24" --lang "en" -o dev/mvfw/data/contentphysical/jomsyfashion.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u shoperfashion -s "mvfw OR (Metaverse Fashion Week)" --since "2022-02-23" --until "2022-04-24" --lang "en" -o dev/mvfw/data/contentphysical/shoperfashion.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u realfaithtribe -s "mvfw OR (Metaverse Fashion Week)" --since "2022-02-23" --until "2022-04-24" --lang "en" -o dev/mvfw/data/contentphysical/realfaithtribe.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u fashionweeknyc -s "mvfw OR (Metaverse Fashion Week)" --since "2022-02-23" --until "2022-04-24" --lang "en" -o dev/mvfw/data/contentphysical/fashionweeknyc.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u fashionblebitch -s "mvfw OR (Metaverse Fashion Week)" --since "2022-02-23" --until "2022-04-24" --lang "en" -o dev/mvfw/data/contentphysical/fashionblebitch.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u voguemagazine -s "mvfw OR (Metaverse Fashion Week)" --since "2022-02-23" --until "2022-04-24" --lang "en" -o dev/mvfw/data/contentphysical/voguemagazine.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u thalia -s "mvfw OR (Metaverse Fashion Week)" --since "2022-02-23" --until "2022-04-24" --lang "en" -o dev/mvfw/data/contentphysical/thalia.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u fashionotes -s "mvfw OR (Metaverse Fashion Week)" --since "2022-02-23" --until "2022-04-24" --lang "en" -o dev/mvfw/data/contentphysical/fashionotes.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u fashionatorapp -s "mvfw OR (Metaverse Fashion Week)" --since "2022-02-23" --until "2022-04-24" --lang "en" -o dev/mvfw/data/contentphysical/fashionatorapp.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u sawwadfashion -s "mvfw OR (Metaverse Fashion Week)" --since "2022-02-23" --until "2022-04-24" --lang "en" -o dev/mvfw/data/contentphysical/sawwadfashion.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u voguesingapore -s "mvfw OR (Metaverse Fashion Week)" --since "2022-02-23" --until "2022-04-24" --lang "en" -o dev/mvfw/data/contentphysical/voguesingapore.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u fashionxcrypto -s "mvfw OR (Metaverse Fashion Week)" --since "2022-02-23" --until "2022-04-24" --lang "en" -o dev/mvfw/data/contentphysical/fashionxcrypto.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -s "mvfw OR (Metaverse Fashion Week)" --since "2022-03-23" --until "2022-03-28" --lang "en" -o dev/mvfw/data/timeFrames/tmp5.csv --csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>twint -u tommyhilfiger -s "mvfw OR (Metaverse Fashion Week)" --since "2022-02-23" --until "2022-04-24" --lang "en" -o dev/mvfw/data/brands/tommyhilfiger.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u forever21 -s "mvfw OR (Metaverse Fashion Week)" --since "2022-02-23" --until "2022-04-24" --lang "en" -o dev/mvfw/data/brands/forever21.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u esteelauder -s "mvfw OR (Metaverse Fashion Week)" --since "2022-02-23" --until "2022-04-24" --lang "en" -o dev/mvfw/data/brands/esteelauder.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u KarlLagerfeld -s "mvfw OR (Metaverse Fashion Week)" --since "2022-02-23" --until "2022-04-24" --lang "en" -o dev/mvfw/data/brands/KarlLagerfeld.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u McQueen -s "mvfw OR (Metaverse Fashion Week)" --since "2022-02-23" --until "2022-04-24" --lang "en" -o dev/mvfw/data/brands/McQueen.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u dkny -s "mvfw OR (Metaverse Fashion Week)" --since "2022-02-23" --until "2022-04-24" --lang "en" -o dev/mvfw/data/brands/dkny.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u dressxcom -s "mvfw OR (Metaverse Fashion Week)" --since "2022-02-23" --until "2022-04-24" --lang "en" -o dev/mvfw/data/brands/dressxcom.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u dolcegabbana -s "mvfw OR (Metaverse Fashion Week)" --since "2022-02-23" --until "2022-04-24" --lang "en" -o dev/mvfw/data/brands/dolcegabbana.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u EtroOfficial -s "mvfw OR (Metaverse Fashion Week)" --since "2022-02-23" --until "2022-04-24" --lang "en" -o dev/mvfw/data/brands/EtroOfficial.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u FranckMuller -s "mvfw OR (Metaverse Fashion Week)" --since "2022-02-23" --until "2022-04-24" --lang "en" -o dev/mvfw/data/brands/FranckMuller.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u Selfridges -s "mvfw OR (Metaverse Fashion Week)" --since "2022-02-23" --until "2022-04-24" --lang "en" -o dev/mvfw/data/brands/Selfridges.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u Bulova -s "mvfw OR (Metaverse Fashion Week)" --since "2022-02-23" --until "2022-04-24" --lang "en" -o dev/mvfw/data/brands/Bulova.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u PacoRabanne -s "mvfw OR (Metaverse Fashion Week)" --since "2022-02-23" --until "2022-04-24" --lang "en" -o dev/mvfw/data/brands/PacoRabanne.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u ArtistVasarely -s "mvfw OR (Metaverse Fashion Week)" --since "2022-02-23" --until "2022-04-24" --lang "en" -o dev/mvfw/data/brands/ArtistVasarely.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u PUMA -s "mvfw OR (Metaverse Fashion Week)" --since "2022-02-23" --until "2022-04-24" --lang "en" -o dev/mvfw/data/brands/PUMA.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u PerryEllis -s "mvfw OR (Metaverse Fashion Week)" --since "2022-02-23" --until "2022-04-24" --lang "en" -o dev/mvfw/data/brands/PerryEllis.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u Fred_Segal -s "mvfw OR (Metaverse Fashion Week)" --since "2022-02-23" --until "2022-04-24" --lang "en" -o dev/mvfw/data/brands/Fred_Segal.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u VAULTswiss -s "mvfw OR (Metaverse Fashion Week)" --since "2022-02-23" --until "2022-04-24" --lang "en" -o dev/mvfw/data/brands/VAULTswiss.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u MissJAlexander -s "mvfw OR (Metaverse Fashion Week)" --since "2022-02-23" --until "2022-04-24" --lang "en" -o dev/mvfw/data/brands/MissJAlexander.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u marc0matic -s "mvfw OR (Metaverse Fashion Week)" --since "2022-02-23" --until "2022-04-24" --lang "en" -o dev/mvfw/data/brands/marc0matic.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u Charles_Keith -s "mvfw OR (Metaverse Fashion Week)" --since "2022-02-23" --until "2022-04-24" --lang "en" -o dev/mvfw/data/brands/Charles_Keith.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u priveporter -s "mvfw OR (Metaverse Fashion Week)" --since "2022-02-23" --until "2022-04-24" --lang "en" -o dev/mvfw/data/brands/priveporter.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u philipp_plein -s "mvfw OR (Metaverse Fashion Week)" --since "2022-02-23" --until "2022-04-24" --lang "en" -o dev/mvfw/data/brands/philipp_plein.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u ElieSaabWorld -s "mvfw OR (Metaverse Fashion Week)" --since "2022-02-23" --until "2022-04-24" --lang "en" -o dev/mvfw/data/brands/ElieSaabWorld.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u HoganBrand -s "mvfw OR (Metaverse Fashion Week)" --since "2022-02-23" --until "2022-04-24" --lang "en" -o dev/mvfw/data/brands/HoganBrand.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u IOCNFTs -s "mvfw OR (Metaverse Fashion Week)" --since "2022-02-23" --until "2022-04-24" --lang "en" -o dev/mvfw/data/brands/IOCNFTs.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -u dundaslondon -s "mvfw OR (Metaverse Fashion Week)" --since "2022-02-23" --until "2022-04-24" --lang "en" -o dev/mvfw/data/brands/dundaslondon.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -s "mvfw OR (Metaverse Fashion Week)" --since "2022-02-23" --until "2022-03-02" --lang "en" -o dev/mvfw/data/timeFrames/tmp1.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -s "mvfw OR (Metaverse Fashion Week)" --since "2022-03-02" --until "2022-03-09" --lang "en" -o dev/mvfw/data/timeFrames/tmp2.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -s "mvfw OR (Metaverse Fashion Week)" --since "2022-03-09" --until "2022-03-16" --lang "en" -o dev/mvfw/data/timeFrames/tmp3.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -s "mvfw OR (Metaverse Fashion Week)" --since "2022-03-16" --until "2022-03-23" --lang "en" -o dev/mvfw/data/timeFrames/tmp4.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -s "mvfw OR (Metaverse Fashion Week)" --since "2022-03-28" --until "2022-04-04" --lang "en" -o dev/mvfw/data/timeFrames/tmp6.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -s "mvfw OR (Metaverse Fashion Week)" --since "2022-04-04" --until "2022-04-11" --lang "en" -o dev/mvfw/data/timeFrames/tmp7.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -s "mvfw OR (Metaverse Fashion Week)" --since "2022-04-11" --until "2022-04-18" --lang "en" -o dev/mvfw/data/timeFrames/tmp8.csv --csv</t>
+  </si>
+  <si>
+    <t>twint -s "mvfw OR (Metaverse Fashion Week)" --since "2022-04-18" --until "2022-04-27" --lang "en" -o dev/mvfw/data/timeFrames/tmp9.csv --csv</t>
+  </si>
+  <si>
+    <t>query</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -252,6 +619,12 @@
       <family val="2"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF333333"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -274,11 +647,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -301,13 +675,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
@@ -349,13 +723,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>317500</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>622300</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
@@ -397,13 +771,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>635000</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>114300</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
@@ -445,13 +819,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>127000</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>431800</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
@@ -493,13 +867,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>444500</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>749300</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
@@ -841,13 +1215,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E09600C-6912-B84E-BE66-88E05D3E2372}">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="2" max="2" width="13.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="137.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -861,242 +1238,1218 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
+      <c r="C2" s="1" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
+      <c r="C3" s="1" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>9</v>
+      <c r="C4" s="1" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>11</v>
+      <c r="C5" s="1" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>13</v>
+      <c r="C6" s="1" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>19</v>
+      <c r="C8" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>21</v>
+      <c r="C9" s="1" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>23</v>
+      <c r="C10" s="1" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>25</v>
+      <c r="C11" s="1" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>29</v>
+      <c r="C14" s="1" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>31</v>
+      <c r="C15" s="1" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>34</v>
+      <c r="C17" s="1" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>36</v>
+      <c r="C18" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>38</v>
+      <c r="C19" s="1" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>40</v>
+      <c r="C20" s="1" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>42</v>
+      <c r="C21" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>58</v>
+        <v>143</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>44</v>
+      <c r="C22" s="1" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>46</v>
+      <c r="C23" s="1" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>48</v>
+      <c r="C24" s="1" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>50</v>
+      <c r="C25" s="1" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>52</v>
+      <c r="C26" s="1" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="C27" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D27" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E27" s="2" t="s">
-        <v>55</v>
+      <c r="E27" s="1" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>57</v>
+      <c r="C28" s="1" t="s">
+        <v>170</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E8" r:id="rId1" display="https://t.co/JUTPHehOWa" xr:uid="{BF6B10CE-729B-454A-8B7C-C324A776D959}"/>
+    <hyperlink ref="D8" r:id="rId1" display="https://t.co/JUTPHehOWa" xr:uid="{BF6B10CE-729B-454A-8B7C-C324A776D959}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38C41DAA-12A9-C749-8EE8-86F787E277D1}">
+  <dimension ref="B1:B10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>178</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E45F79AE-9AB3-8E4E-92FB-F32E507820DA}">
+  <dimension ref="A1:C28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="139.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD71864D-CA6C-E14D-AF82-ED7BF0980D6C}">
+  <dimension ref="A1:C28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="105.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" t="s">
+        <v>111</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EF826CF-E9FA-9F4A-AD62-09A59C7C56F3}">
+  <dimension ref="A1:A30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="225.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="20" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="20" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="20" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="20" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="20" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="20" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="20" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="20" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="20" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="20" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="20" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="20" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="20" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="20" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" ht="20" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" ht="20" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="20" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="20" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="20" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="20" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="20" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" ht="20" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" ht="20" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" ht="20" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" ht="20" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" ht="20" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" ht="20" x14ac:dyDescent="0.2">
+      <c r="A27" s="4" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" ht="20" x14ac:dyDescent="0.2">
+      <c r="A28" s="4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" ht="20" x14ac:dyDescent="0.2">
+      <c r="A29" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" ht="20" x14ac:dyDescent="0.2">
+      <c r="A30" s="4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>